<commit_message>
Manual Match window functioning, but not updating report Added new plan data sources
</commit_message>
<xml_diff>
--- a/Test Data/Printout Data/Variables.xlsx
+++ b/Test Data/Printout Data/Variables.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Python\Projects\EclipseRelated\PlanEvaluation\Test Data\Printout Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_DE130BD1D66E607F3BA5E3CE813341BCBA2F07BA" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="27555" windowHeight="12045"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,15 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -622,7 +636,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -663,6 +677,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1374,7 +1391,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1407,9 +1424,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1442,6 +1476,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1617,11 +1668,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>